<commit_message>
Improve IO Control testbench
</commit_message>
<xml_diff>
--- a/doc/Time Records.xlsx
+++ b/doc/Time Records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\dse\calculator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B22E55A-42A1-46E7-B9A6-64BFAB18B5C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55640EF-1274-4550-9BAB-015A6E20982F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15390" windowHeight="9533" xr2:uid="{24B1E086-FE3D-4C8E-9000-B7596E70FAC3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{24B1E086-FE3D-4C8E-9000-B7596E70FAC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>18.11.2019</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Architecture, Testbench</t>
+  </si>
+  <si>
+    <t>Testbench</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EA29A6-C5C6-4E60-8E49-CEF8CCBA1158}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -465,7 +468,7 @@
         <v>0.46527777777777773</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D6" si="0">C2-B2</f>
+        <f t="shared" ref="D2:D7" si="0">C2-B2</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E2" t="s">
@@ -557,6 +560,27 @@
       </c>
       <c r="F6" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a enum type for operations for simulations
</commit_message>
<xml_diff>
--- a/doc/Time Records.xlsx
+++ b/doc/Time Records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\dse\calculator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55640EF-1274-4550-9BAB-015A6E20982F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3612A622-FCED-484B-AA29-F68D2144C7EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{24B1E086-FE3D-4C8E-9000-B7596E70FAC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>18.11.2019</t>
   </si>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EA29A6-C5C6-4E60-8E49-CEF8CCBA1158}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -468,7 +468,7 @@
         <v>0.46527777777777773</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D7" si="0">C2-B2</f>
+        <f t="shared" ref="D2:D8" si="0">C2-B2</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E2" t="s">
@@ -581,6 +581,27 @@
       </c>
       <c r="F7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Architecture and testbench of ALU unit
</commit_message>
<xml_diff>
--- a/doc/Time Records.xlsx
+++ b/doc/Time Records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\dse\calculator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3612A622-FCED-484B-AA29-F68D2144C7EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4E72B5-34C6-4646-9F49-05B3A84B2228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{24B1E086-FE3D-4C8E-9000-B7596E70FAC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>18.11.2019</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Testbench</t>
+  </si>
+  <si>
+    <t>27.11.2019</t>
+  </si>
+  <si>
+    <t>ALU Unit</t>
   </si>
 </sst>
 </file>
@@ -423,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EA29A6-C5C6-4E60-8E49-CEF8CCBA1158}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -468,7 +474,7 @@
         <v>0.46527777777777773</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D8" si="0">C2-B2</f>
+        <f t="shared" ref="D2:D9" si="0">C2-B2</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E2" t="s">
@@ -601,6 +607,27 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add architecture and testbench of Top Unit
</commit_message>
<xml_diff>
--- a/doc/Time Records.xlsx
+++ b/doc/Time Records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\dse\calculator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4E72B5-34C6-4646-9F49-05B3A84B2228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C617A05-D809-4A3C-A819-1E2ECA433832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{24B1E086-FE3D-4C8E-9000-B7596E70FAC3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24B1E086-FE3D-4C8E-9000-B7596E70FAC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>18.11.2019</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>ALU Unit</t>
+  </si>
+  <si>
+    <t>29.11.2019</t>
+  </si>
+  <si>
+    <t>Top Unit</t>
   </si>
 </sst>
 </file>
@@ -117,7 +123,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -133,7 +139,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -429,20 +435,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EA29A6-C5C6-4E60-8E49-CEF8CCBA1158}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -474,7 +480,7 @@
         <v>0.46527777777777773</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D9" si="0">C2-B2</f>
+        <f t="shared" ref="D2:D10" si="0">C2-B2</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E2" t="s">
@@ -484,7 +490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -505,7 +511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -526,7 +532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -547,7 +553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -568,7 +574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -589,7 +595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -610,7 +616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -628,6 +634,27 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Comment IO Control Unit
</commit_message>
<xml_diff>
--- a/doc/Time Records.xlsx
+++ b/doc/Time Records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\dse\calculator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C617A05-D809-4A3C-A819-1E2ECA433832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42917A69-3209-4279-B97C-01FDDAB5A54A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24B1E086-FE3D-4C8E-9000-B7596E70FAC3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{24B1E086-FE3D-4C8E-9000-B7596E70FAC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>18.11.2019</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Top Unit</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -139,7 +142,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -435,20 +438,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EA29A6-C5C6-4E60-8E49-CEF8CCBA1158}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -480,7 +483,7 @@
         <v>0.46527777777777773</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D10" si="0">C2-B2</f>
+        <f t="shared" ref="D2:D11" si="0">C2-B2</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E2" t="s">
@@ -490,7 +493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -511,7 +514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -532,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -553,7 +556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -574,7 +577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -595,7 +598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -616,7 +619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -637,7 +640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -656,6 +659,27 @@
       </c>
       <c r="F10" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comment Calculator Control architecture
</commit_message>
<xml_diff>
--- a/doc/Time Records.xlsx
+++ b/doc/Time Records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\technikum\dse\calculator\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42917A69-3209-4279-B97C-01FDDAB5A54A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7EB579-6183-443F-AEE8-CCB187403FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{24B1E086-FE3D-4C8E-9000-B7596E70FAC3}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{24B1E086-FE3D-4C8E-9000-B7596E70FAC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>18.11.2019</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>30.11.2019</t>
+  </si>
+  <si>
+    <t>Commenting</t>
   </si>
 </sst>
 </file>
@@ -126,7 +132,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -142,7 +148,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -438,20 +444,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EA29A6-C5C6-4E60-8E49-CEF8CCBA1158}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -483,7 +489,7 @@
         <v>0.46527777777777773</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D11" si="0">C2-B2</f>
+        <f t="shared" ref="D2:D12" si="0">C2-B2</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E2" t="s">
@@ -493,7 +499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -514,7 +520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -535,7 +541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -556,7 +562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -577,7 +583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -598,7 +604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -619,7 +625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -640,7 +646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -661,7 +667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -680,6 +686,27 @@
       </c>
       <c r="F11" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>